<commit_message>
correct status details for bmi and med_diabetes
</commit_message>
<xml_diff>
--- a/data_processing_elements-CHS.xlsx
+++ b/data_processing_elements-CHS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CADF4E-F02E-45A4-BF65-F76DAD75A65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564F4A51-9DC4-416E-8AB1-2A50BA004A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1655,7 +1655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1713,9 +1713,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2059,10 +2056,10 @@
   <dimension ref="A1:U84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R7" sqref="R7"/>
+      <selection pane="bottomRight" activeCell="O56" sqref="O56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3077,7 +3074,7 @@
         <v>25</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="R20" s="3" t="s">
         <v>44</v>
@@ -4218,7 +4215,7 @@
       <c r="S43" s="21" t="s">
         <v>415</v>
       </c>
-      <c r="T43" s="22"/>
+      <c r="T43" s="3"/>
       <c r="U43" s="3"/>
     </row>
     <row r="44" spans="1:21" ht="370.5" x14ac:dyDescent="0.25">
@@ -4899,7 +4896,7 @@
         <v>25</v>
       </c>
       <c r="Q57" s="3" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="R57" s="3" t="s">
         <v>204</v>

</xml_diff>

<commit_message>
Modify the id variable name
</commit_message>
<xml_diff>
--- a/data_processing_elements-CHS.xlsx
+++ b/data_processing_elements-CHS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maelstrom\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7785784A-CD55-42AD-A093-DB600E1BAAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F66206E-B8AD-4495-A810-0BAA59F5F05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="465" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="420">
   <si>
     <t>index</t>
   </si>
@@ -1531,6 +1531,9 @@
   </si>
   <si>
     <t>k0alder5</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -1643,7 +1646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1689,9 +1692,8 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2040,37 +2042,37 @@
   <dimension ref="A1:U84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K48" sqref="K48"/>
+      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="2"/>
-    <col min="8" max="8" width="8.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="36.7109375" style="10" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="26.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="30.140625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="31.85546875" style="10" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="21.28515625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" style="18" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" style="18" customWidth="1"/>
-    <col min="18" max="18" width="17.5703125" style="18" customWidth="1"/>
-    <col min="19" max="19" width="19.85546875" style="18" customWidth="1"/>
-    <col min="20" max="21" width="9.140625" style="2"/>
+    <col min="1" max="1" width="4.7265625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.26953125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30.54296875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.453125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" style="2"/>
+    <col min="8" max="8" width="8.54296875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="36.7265625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="25.1796875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="26.453125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="30.1796875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="31.81640625" style="10" customWidth="1"/>
+    <col min="14" max="14" width="7.7265625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="21.26953125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="12.7265625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="12.453125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="17.54296875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="19.81640625" style="2" customWidth="1"/>
+    <col min="20" max="21" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2135,7 +2137,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2158,7 +2160,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="9"/>
       <c r="J2" s="12" t="s">
-        <v>289</v>
+        <v>419</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>290</v>
@@ -2166,22 +2168,22 @@
       <c r="L2" s="3"/>
       <c r="M2" s="9"/>
       <c r="N2" s="3"/>
-      <c r="P2" s="18" t="s">
+      <c r="P2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="18" t="s">
+      <c r="Q2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R2" s="18" t="s">
+      <c r="R2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="S2" s="18" t="s">
+      <c r="S2" s="2" t="s">
         <v>289</v>
       </c>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2214,22 +2216,22 @@
       <c r="L3" s="3"/>
       <c r="M3" s="9"/>
       <c r="N3" s="3"/>
-      <c r="P3" s="18" t="s">
+      <c r="P3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q3" s="18" t="s">
+      <c r="Q3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R3" s="18" t="s">
+      <c r="R3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="S3" s="19" t="s">
+      <c r="S3" s="18" t="s">
         <v>413</v>
       </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
     </row>
-    <row r="4" spans="1:21" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2264,22 +2266,22 @@
         <v>294</v>
       </c>
       <c r="N4" s="3"/>
-      <c r="P4" s="18" t="s">
+      <c r="P4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" s="18" t="s">
+      <c r="Q4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="18" t="s">
+      <c r="R4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S4" s="18" t="s">
+      <c r="S4" s="2" t="s">
         <v>295</v>
       </c>
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
     </row>
-    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2310,22 +2312,22 @@
       <c r="L5" s="3"/>
       <c r="M5" s="9"/>
       <c r="N5" s="3"/>
-      <c r="P5" s="20" t="s">
+      <c r="P5" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="Q5" s="18" t="s">
+      <c r="Q5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R5" s="21" t="s">
+      <c r="R5" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="S5" s="21" t="s">
+      <c r="S5" s="20" t="s">
         <v>44</v>
       </c>
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
     </row>
-    <row r="6" spans="1:21" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2362,22 +2364,22 @@
         <v>299</v>
       </c>
       <c r="N6" s="3"/>
-      <c r="P6" s="18" t="s">
+      <c r="P6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q6" s="18" t="s">
+      <c r="Q6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R6" s="18" t="s">
+      <c r="R6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S6" s="18" t="s">
+      <c r="S6" s="2" t="s">
         <v>414</v>
       </c>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
     </row>
-    <row r="7" spans="1:21" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="112.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2412,16 +2414,16 @@
         <v>302</v>
       </c>
       <c r="N7" s="3"/>
-      <c r="P7" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q7" s="18" t="s">
+      <c r="P7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q7" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="R7" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S7" s="18" t="s">
+      <c r="R7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S7" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T7" s="15" t="s">
@@ -2429,7 +2431,7 @@
       </c>
       <c r="U7" s="3"/>
     </row>
-    <row r="8" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="25" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2460,16 +2462,16 @@
       <c r="L8" s="3"/>
       <c r="M8" s="9"/>
       <c r="N8" s="3"/>
-      <c r="P8" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q8" s="18" t="s">
+      <c r="P8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R8" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S8" s="18" t="s">
+      <c r="R8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S8" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T8" s="15" t="s">
@@ -2477,7 +2479,7 @@
       </c>
       <c r="U8" s="3"/>
     </row>
-    <row r="9" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="25" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2508,22 +2510,22 @@
       <c r="L9" s="3"/>
       <c r="M9" s="9"/>
       <c r="N9" s="3"/>
-      <c r="P9" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q9" s="18" t="s">
+      <c r="P9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R9" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S9" s="18" t="s">
+      <c r="R9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S9" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2552,22 +2554,22 @@
       <c r="L10" s="3"/>
       <c r="M10" s="9"/>
       <c r="N10" s="3"/>
-      <c r="P10" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q10" s="18" t="s">
+      <c r="P10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R10" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S10" s="18" t="s">
+      <c r="R10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S10" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2596,16 +2598,16 @@
       <c r="L11" s="3"/>
       <c r="M11" s="9"/>
       <c r="N11" s="3"/>
-      <c r="P11" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q11" s="18" t="s">
+      <c r="P11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q11" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="R11" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S11" s="18" t="s">
+      <c r="R11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S11" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T11" s="3" t="s">
@@ -2613,7 +2615,7 @@
       </c>
       <c r="U11" s="3"/>
     </row>
-    <row r="12" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="25" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2644,22 +2646,22 @@
       <c r="L12" s="3"/>
       <c r="M12" s="9"/>
       <c r="N12" s="3"/>
-      <c r="P12" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q12" s="18" t="s">
+      <c r="P12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R12" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S12" s="18" t="s">
+      <c r="R12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S12" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
     </row>
-    <row r="13" spans="1:21" ht="51" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="50" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2693,22 +2695,22 @@
       <c r="M13" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="P13" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q13" s="18" t="s">
+      <c r="P13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q13" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="R13" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S13" s="18" t="s">
+      <c r="R13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S13" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
     </row>
-    <row r="14" spans="1:21" ht="51" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="50" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2742,22 +2744,22 @@
       <c r="M14" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="P14" s="18" t="s">
+      <c r="P14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q14" s="18" t="s">
+      <c r="Q14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R14" s="18" t="s">
+      <c r="R14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S14" s="18" t="s">
+      <c r="S14" s="2" t="s">
         <v>309</v>
       </c>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
     </row>
-    <row r="15" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="25" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2788,16 +2790,16 @@
       <c r="L15" s="3"/>
       <c r="M15" s="9"/>
       <c r="N15" s="3"/>
-      <c r="P15" s="18" t="s">
+      <c r="P15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q15" s="18" t="s">
+      <c r="Q15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R15" s="18" t="s">
+      <c r="R15" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="S15" s="18">
+      <c r="S15" s="2">
         <v>2</v>
       </c>
       <c r="T15" s="15" t="s">
@@ -2805,7 +2807,7 @@
       </c>
       <c r="U15" s="3"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2842,22 +2844,22 @@
       <c r="N16" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="P16" s="18" t="s">
+      <c r="P16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q16" s="18" t="s">
+      <c r="Q16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R16" s="18" t="s">
+      <c r="R16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S16" s="18" t="s">
+      <c r="S16" s="2" t="s">
         <v>44</v>
       </c>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
     </row>
-    <row r="17" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="25" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2894,16 +2896,16 @@
       <c r="N17" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="P17" s="18" t="s">
+      <c r="P17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q17" s="18" t="s">
+      <c r="Q17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R17" s="18" t="s">
+      <c r="R17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="S17" s="18" t="s">
+      <c r="S17" s="2" t="s">
         <v>314</v>
       </c>
       <c r="T17" s="15" t="s">
@@ -2911,7 +2913,7 @@
       </c>
       <c r="U17" s="3"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2948,22 +2950,22 @@
       <c r="N18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="P18" s="18" t="s">
+      <c r="P18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q18" s="18" t="s">
+      <c r="Q18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R18" s="18" t="s">
+      <c r="R18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S18" s="18" t="s">
+      <c r="S18" s="2" t="s">
         <v>44</v>
       </c>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
     </row>
-    <row r="19" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="25" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -3000,16 +3002,16 @@
       <c r="N19" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="P19" s="18" t="s">
+      <c r="P19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q19" s="18" t="s">
+      <c r="Q19" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R19" s="18" t="s">
+      <c r="R19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="S19" s="18" t="s">
+      <c r="S19" s="2" t="s">
         <v>319</v>
       </c>
       <c r="T19" s="15" t="s">
@@ -3017,7 +3019,7 @@
       </c>
       <c r="U19" s="3"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -3052,22 +3054,22 @@
       <c r="N20" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="P20" s="18" t="s">
+      <c r="P20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q20" s="18" t="s">
+      <c r="Q20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R20" s="18" t="s">
+      <c r="R20" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S20" s="18" t="s">
+      <c r="S20" s="2" t="s">
         <v>44</v>
       </c>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -3104,22 +3106,22 @@
       <c r="N21" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="P21" s="18" t="s">
+      <c r="P21" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q21" s="18" t="s">
+      <c r="Q21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R21" s="18" t="s">
+      <c r="R21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S21" s="18" t="s">
+      <c r="S21" s="2" t="s">
         <v>44</v>
       </c>
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
     </row>
-    <row r="22" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="25" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -3156,22 +3158,22 @@
       <c r="N22" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="P22" s="18" t="s">
+      <c r="P22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q22" s="18" t="s">
+      <c r="Q22" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R22" s="18" t="s">
+      <c r="R22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="S22" s="18" t="s">
+      <c r="S22" s="2" t="s">
         <v>325</v>
       </c>
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -3202,22 +3204,22 @@
       <c r="L23" s="3"/>
       <c r="M23" s="9"/>
       <c r="N23" s="3"/>
-      <c r="P23" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q23" s="18" t="s">
+      <c r="P23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q23" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R23" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S23" s="18" t="s">
+      <c r="R23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S23" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -3246,22 +3248,22 @@
       <c r="L24" s="3"/>
       <c r="M24" s="9"/>
       <c r="N24" s="3"/>
-      <c r="P24" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q24" s="18" t="s">
+      <c r="P24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q24" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R24" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S24" s="18" t="s">
+      <c r="R24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S24" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
     </row>
-    <row r="25" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -3301,22 +3303,22 @@
       <c r="O25" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="P25" s="18" t="s">
+      <c r="P25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q25" s="18" t="s">
+      <c r="Q25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R25" s="18" t="s">
+      <c r="R25" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="S25" s="18" t="s">
+      <c r="S25" s="2" t="s">
         <v>416</v>
       </c>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
     </row>
-    <row r="26" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -3356,22 +3358,22 @@
       <c r="O26" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="P26" s="18" t="s">
+      <c r="P26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q26" s="18" t="s">
+      <c r="Q26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R26" s="18" t="s">
+      <c r="R26" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="S26" s="18" t="s">
+      <c r="S26" s="2" t="s">
         <v>417</v>
       </c>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -3402,22 +3404,22 @@
       <c r="L27" s="3"/>
       <c r="M27" s="9"/>
       <c r="N27" s="3"/>
-      <c r="P27" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q27" s="18" t="s">
+      <c r="P27" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q27" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R27" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S27" s="18" t="s">
+      <c r="R27" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S27" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T27" s="3"/>
       <c r="U27" s="3"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -3448,22 +3450,22 @@
       <c r="L28" s="3"/>
       <c r="M28" s="9"/>
       <c r="N28" s="3"/>
-      <c r="P28" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q28" s="18" t="s">
+      <c r="P28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R28" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S28" s="18" t="s">
+      <c r="R28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S28" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
     </row>
-    <row r="29" spans="1:21" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="112.5" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -3500,22 +3502,22 @@
         <v>333</v>
       </c>
       <c r="N29" s="3"/>
-      <c r="P29" s="18" t="s">
+      <c r="P29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q29" s="18" t="s">
+      <c r="Q29" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R29" s="18" t="s">
+      <c r="R29" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S29" s="18" t="s">
+      <c r="S29" s="2" t="s">
         <v>334</v>
       </c>
       <c r="T29" s="3"/>
       <c r="U29" s="3"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -3548,16 +3550,16 @@
       <c r="L30" s="3"/>
       <c r="M30" s="9"/>
       <c r="N30" s="3"/>
-      <c r="P30" s="18" t="s">
+      <c r="P30" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q30" s="18" t="s">
+      <c r="Q30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R30" s="18" t="s">
+      <c r="R30" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S30" s="18" t="s">
+      <c r="S30" s="2" t="s">
         <v>44</v>
       </c>
       <c r="T30" s="15" t="s">
@@ -3565,7 +3567,7 @@
       </c>
       <c r="U30" s="3"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -3596,22 +3598,22 @@
       <c r="L31" s="3"/>
       <c r="M31" s="9"/>
       <c r="N31" s="3"/>
-      <c r="P31" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q31" s="18" t="s">
+      <c r="P31" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q31" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R31" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S31" s="18" t="s">
+      <c r="R31" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S31" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T31" s="3"/>
       <c r="U31" s="3"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -3646,22 +3648,22 @@
       <c r="N32" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="P32" s="18" t="s">
+      <c r="P32" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q32" s="18" t="s">
+      <c r="Q32" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R32" s="18" t="s">
+      <c r="R32" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S32" s="18" t="s">
+      <c r="S32" s="2" t="s">
         <v>44</v>
       </c>
       <c r="T32" s="3"/>
       <c r="U32" s="3"/>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -3694,16 +3696,16 @@
       <c r="L33" s="3"/>
       <c r="M33" s="9"/>
       <c r="N33" s="3"/>
-      <c r="P33" s="18" t="s">
+      <c r="P33" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q33" s="18" t="s">
+      <c r="Q33" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R33" s="18" t="s">
+      <c r="R33" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S33" s="18" t="s">
+      <c r="S33" s="2" t="s">
         <v>44</v>
       </c>
       <c r="T33" s="15" t="s">
@@ -3711,7 +3713,7 @@
       </c>
       <c r="U33" s="3"/>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -3746,22 +3748,22 @@
       <c r="N34" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="P34" s="18" t="s">
+      <c r="P34" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q34" s="18" t="s">
+      <c r="Q34" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R34" s="18" t="s">
+      <c r="R34" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S34" s="18" t="s">
+      <c r="S34" s="2" t="s">
         <v>44</v>
       </c>
       <c r="T34" s="3"/>
       <c r="U34" s="3"/>
     </row>
-    <row r="35" spans="1:21" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -3799,22 +3801,22 @@
       <c r="O35" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="P35" s="18" t="s">
+      <c r="P35" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q35" s="18" t="s">
+      <c r="Q35" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R35" s="18" t="s">
+      <c r="R35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="S35" s="18" t="s">
+      <c r="S35" s="2" t="s">
         <v>348</v>
       </c>
       <c r="T35" s="3"/>
       <c r="U35" s="3"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -3849,22 +3851,22 @@
       <c r="N36" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="P36" s="18" t="s">
+      <c r="P36" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q36" s="18" t="s">
+      <c r="Q36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R36" s="18" t="s">
+      <c r="R36" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S36" s="18" t="s">
+      <c r="S36" s="2" t="s">
         <v>44</v>
       </c>
       <c r="T36" s="3"/>
       <c r="U36" s="3"/>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -3899,22 +3901,22 @@
       <c r="N37" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="P37" s="18" t="s">
+      <c r="P37" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q37" s="18" t="s">
+      <c r="Q37" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R37" s="18" t="s">
+      <c r="R37" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S37" s="18" t="s">
+      <c r="S37" s="2" t="s">
         <v>44</v>
       </c>
       <c r="T37" s="3"/>
       <c r="U37" s="3"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -3945,22 +3947,22 @@
       <c r="L38" s="3"/>
       <c r="M38" s="9"/>
       <c r="N38" s="3"/>
-      <c r="P38" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q38" s="18" t="s">
+      <c r="P38" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q38" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R38" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S38" s="18" t="s">
+      <c r="R38" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S38" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T38" s="3"/>
       <c r="U38" s="3"/>
     </row>
-    <row r="39" spans="1:21" ht="102" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="100" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -3995,22 +3997,22 @@
         <v>356</v>
       </c>
       <c r="N39" s="3"/>
-      <c r="P39" s="18" t="s">
+      <c r="P39" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q39" s="18" t="s">
+      <c r="Q39" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R39" s="18" t="s">
+      <c r="R39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S39" s="18" t="s">
+      <c r="S39" s="2" t="s">
         <v>357</v>
       </c>
       <c r="T39" s="3"/>
       <c r="U39" s="3"/>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -4041,22 +4043,22 @@
       <c r="L40" s="3"/>
       <c r="M40" s="9"/>
       <c r="N40" s="3"/>
-      <c r="P40" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q40" s="18" t="s">
+      <c r="P40" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q40" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R40" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S40" s="18" t="s">
+      <c r="R40" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S40" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T40" s="3"/>
       <c r="U40" s="3"/>
     </row>
-    <row r="41" spans="1:21" ht="102" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" ht="100" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -4091,22 +4093,22 @@
         <v>356</v>
       </c>
       <c r="N41" s="3"/>
-      <c r="P41" s="18" t="s">
+      <c r="P41" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q41" s="18" t="s">
+      <c r="Q41" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R41" s="18" t="s">
+      <c r="R41" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S41" s="18" t="s">
+      <c r="S41" s="2" t="s">
         <v>357</v>
       </c>
       <c r="T41" s="3"/>
       <c r="U41" s="3"/>
     </row>
-    <row r="42" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -4137,22 +4139,22 @@
       <c r="L42" s="3"/>
       <c r="M42" s="9"/>
       <c r="N42" s="3"/>
-      <c r="P42" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q42" s="18" t="s">
+      <c r="P42" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q42" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R42" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S42" s="18" t="s">
+      <c r="R42" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S42" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T42" s="3"/>
       <c r="U42" s="3"/>
     </row>
-    <row r="43" spans="1:21" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" ht="71" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -4200,7 +4202,7 @@
       <c r="T43" s="3"/>
       <c r="U43" s="3"/>
     </row>
-    <row r="44" spans="1:21" ht="371.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="322.5" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -4235,13 +4237,13 @@
         <v>364</v>
       </c>
       <c r="N44" s="3"/>
-      <c r="P44" s="18" t="s">
+      <c r="P44" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q44" s="18" t="s">
+      <c r="Q44" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R44" s="18" t="s">
+      <c r="R44" s="2" t="s">
         <v>204</v>
       </c>
       <c r="S44" s="1" t="s">
@@ -4250,7 +4252,7 @@
       <c r="T44" s="3"/>
       <c r="U44" s="3"/>
     </row>
-    <row r="45" spans="1:21" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="112.5" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -4285,13 +4287,13 @@
         <v>368</v>
       </c>
       <c r="N45" s="3"/>
-      <c r="P45" s="18" t="s">
+      <c r="P45" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q45" s="18" t="s">
+      <c r="Q45" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R45" s="18" t="s">
+      <c r="R45" s="2" t="s">
         <v>204</v>
       </c>
       <c r="S45" s="1" t="s">
@@ -4300,7 +4302,7 @@
       <c r="T45" s="3"/>
       <c r="U45" s="3"/>
     </row>
-    <row r="46" spans="1:21" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -4336,21 +4338,21 @@
       </c>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
-      <c r="P46" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q46" s="18" t="s">
+      <c r="P46" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q46" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R46" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S46" s="18" t="s">
+      <c r="R46" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S46" s="2" t="s">
         <v>59</v>
       </c>
       <c r="U46" s="3"/>
     </row>
-    <row r="47" spans="1:21" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -4383,22 +4385,22 @@
       </c>
       <c r="M47" s="9"/>
       <c r="N47" s="3"/>
-      <c r="P47" s="18" t="s">
+      <c r="P47" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q47" s="18" t="s">
+      <c r="Q47" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R47" s="18" t="s">
+      <c r="R47" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="S47" s="18" t="s">
+      <c r="S47" s="2" t="s">
         <v>372</v>
       </c>
       <c r="T47" s="3"/>
       <c r="U47" s="3"/>
     </row>
-    <row r="48" spans="1:21" ht="51" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="50" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -4429,22 +4431,22 @@
       <c r="L48" s="3"/>
       <c r="M48" s="9"/>
       <c r="N48" s="3"/>
-      <c r="P48" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q48" s="18" t="s">
+      <c r="P48" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q48" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R48" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S48" s="18" t="s">
+      <c r="R48" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S48" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T48" s="3"/>
       <c r="U48" s="3"/>
     </row>
-    <row r="49" spans="1:21" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" ht="112.5" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -4479,13 +4481,13 @@
         <v>368</v>
       </c>
       <c r="N49" s="3"/>
-      <c r="P49" s="18" t="s">
+      <c r="P49" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q49" s="18" t="s">
+      <c r="Q49" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R49" s="18" t="s">
+      <c r="R49" s="2" t="s">
         <v>204</v>
       </c>
       <c r="S49" s="1" t="s">
@@ -4494,7 +4496,7 @@
       <c r="T49" s="3"/>
       <c r="U49" s="3"/>
     </row>
-    <row r="50" spans="1:21" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" ht="56.5" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -4529,13 +4531,13 @@
         <v>368</v>
       </c>
       <c r="N50" s="3"/>
-      <c r="P50" s="18" t="s">
+      <c r="P50" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q50" s="18" t="s">
+      <c r="Q50" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R50" s="18" t="s">
+      <c r="R50" s="2" t="s">
         <v>204</v>
       </c>
       <c r="S50" s="1" t="s">
@@ -4544,7 +4546,7 @@
       <c r="T50" s="3"/>
       <c r="U50" s="3"/>
     </row>
-    <row r="51" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" ht="25" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -4582,22 +4584,22 @@
       <c r="O51" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="P51" s="18" t="s">
+      <c r="P51" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q51" s="18" t="s">
+      <c r="Q51" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R51" s="18" t="s">
+      <c r="R51" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S51" s="18" t="s">
+      <c r="S51" s="2" t="s">
         <v>194</v>
       </c>
       <c r="T51" s="3"/>
       <c r="U51" s="3"/>
     </row>
-    <row r="52" spans="1:21" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -4628,22 +4630,22 @@
       <c r="L52" s="3"/>
       <c r="M52" s="9"/>
       <c r="N52" s="3"/>
-      <c r="P52" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q52" s="18" t="s">
+      <c r="P52" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q52" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R52" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S52" s="18" t="s">
+      <c r="R52" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S52" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T52" s="3"/>
       <c r="U52" s="3"/>
     </row>
-    <row r="53" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" ht="25" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -4678,22 +4680,22 @@
         <v>368</v>
       </c>
       <c r="N53" s="3"/>
-      <c r="P53" s="18" t="s">
+      <c r="P53" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q53" s="18" t="s">
+      <c r="Q53" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R53" s="18" t="s">
+      <c r="R53" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S53" s="18" t="s">
+      <c r="S53" s="2" t="s">
         <v>194</v>
       </c>
       <c r="T53" s="3"/>
       <c r="U53" s="3"/>
     </row>
-    <row r="54" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="25" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -4724,22 +4726,22 @@
       <c r="L54" s="3"/>
       <c r="M54" s="9"/>
       <c r="N54" s="3"/>
-      <c r="P54" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q54" s="18" t="s">
+      <c r="P54" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q54" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R54" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S54" s="18" t="s">
+      <c r="R54" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S54" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T54" s="3"/>
       <c r="U54" s="3"/>
     </row>
-    <row r="55" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" ht="25" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -4774,22 +4776,22 @@
         <v>368</v>
       </c>
       <c r="N55" s="3"/>
-      <c r="P55" s="18" t="s">
+      <c r="P55" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q55" s="18" t="s">
+      <c r="Q55" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R55" s="18" t="s">
+      <c r="R55" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S55" s="18" t="s">
+      <c r="S55" s="2" t="s">
         <v>194</v>
       </c>
       <c r="T55" s="3"/>
       <c r="U55" s="3"/>
     </row>
-    <row r="56" spans="1:21" ht="100.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" ht="84.5" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -4824,13 +4826,13 @@
         <v>368</v>
       </c>
       <c r="N56" s="3"/>
-      <c r="P56" s="18" t="s">
+      <c r="P56" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q56" s="18" t="s">
+      <c r="Q56" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R56" s="18" t="s">
+      <c r="R56" s="2" t="s">
         <v>204</v>
       </c>
       <c r="S56" s="1" t="s">
@@ -4839,7 +4841,7 @@
       <c r="T56" s="3"/>
       <c r="U56" s="3"/>
     </row>
-    <row r="57" spans="1:21" ht="72" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" ht="70.5" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -4874,13 +4876,13 @@
         <v>368</v>
       </c>
       <c r="N57" s="3"/>
-      <c r="P57" s="18" t="s">
+      <c r="P57" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q57" s="18" t="s">
+      <c r="Q57" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R57" s="18" t="s">
+      <c r="R57" s="2" t="s">
         <v>204</v>
       </c>
       <c r="S57" s="1" t="s">
@@ -4889,7 +4891,7 @@
       <c r="T57" s="3"/>
       <c r="U57" s="3"/>
     </row>
-    <row r="58" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" ht="25" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -4920,22 +4922,22 @@
       <c r="L58" s="3"/>
       <c r="M58" s="9"/>
       <c r="N58" s="3"/>
-      <c r="P58" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q58" s="18" t="s">
+      <c r="P58" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q58" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R58" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S58" s="18" t="s">
+      <c r="R58" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S58" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T58" s="3"/>
       <c r="U58" s="3"/>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -4964,22 +4966,22 @@
       <c r="L59" s="3"/>
       <c r="M59" s="9"/>
       <c r="N59" s="3"/>
-      <c r="P59" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q59" s="18" t="s">
+      <c r="P59" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q59" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R59" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S59" s="18" t="s">
+      <c r="R59" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S59" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T59" s="3"/>
       <c r="U59" s="3"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -5008,22 +5010,22 @@
       <c r="L60" s="3"/>
       <c r="M60" s="9"/>
       <c r="N60" s="3"/>
-      <c r="P60" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q60" s="18" t="s">
+      <c r="P60" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q60" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R60" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S60" s="18" t="s">
+      <c r="R60" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S60" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T60" s="3"/>
       <c r="U60" s="3"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -5052,22 +5054,22 @@
       <c r="L61" s="3"/>
       <c r="M61" s="9"/>
       <c r="N61" s="3"/>
-      <c r="P61" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q61" s="18" t="s">
+      <c r="P61" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q61" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R61" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S61" s="18" t="s">
+      <c r="R61" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S61" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T61" s="3"/>
       <c r="U61" s="3"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -5096,22 +5098,22 @@
       <c r="L62" s="3"/>
       <c r="M62" s="9"/>
       <c r="N62" s="3"/>
-      <c r="P62" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q62" s="18" t="s">
+      <c r="P62" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q62" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R62" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S62" s="18" t="s">
+      <c r="R62" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S62" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T62" s="3"/>
       <c r="U62" s="3"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -5140,22 +5142,22 @@
       <c r="L63" s="3"/>
       <c r="M63" s="9"/>
       <c r="N63" s="3"/>
-      <c r="P63" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q63" s="18" t="s">
+      <c r="P63" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q63" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R63" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S63" s="18" t="s">
+      <c r="R63" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S63" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T63" s="3"/>
       <c r="U63" s="3"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -5184,22 +5186,22 @@
       <c r="L64" s="3"/>
       <c r="M64" s="9"/>
       <c r="N64" s="3"/>
-      <c r="P64" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q64" s="18" t="s">
+      <c r="P64" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q64" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R64" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S64" s="18" t="s">
+      <c r="R64" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S64" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T64" s="3"/>
       <c r="U64" s="3"/>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -5228,22 +5230,22 @@
       <c r="L65" s="3"/>
       <c r="M65" s="9"/>
       <c r="N65" s="3"/>
-      <c r="P65" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q65" s="18" t="s">
+      <c r="P65" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q65" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R65" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S65" s="18" t="s">
+      <c r="R65" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S65" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T65" s="3"/>
       <c r="U65" s="3"/>
     </row>
-    <row r="66" spans="1:21" ht="51" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" ht="50" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -5274,22 +5276,22 @@
       <c r="L66" s="3"/>
       <c r="M66" s="9"/>
       <c r="N66" s="3"/>
-      <c r="P66" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q66" s="18" t="s">
+      <c r="P66" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q66" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R66" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S66" s="18" t="s">
+      <c r="R66" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S66" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T66" s="3"/>
       <c r="U66" s="3"/>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -5325,22 +5327,22 @@
       <c r="O67" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="P67" s="18" t="s">
+      <c r="P67" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q67" s="18" t="s">
+      <c r="Q67" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R67" s="18" t="s">
+      <c r="R67" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S67" s="18" t="s">
+      <c r="S67" s="2" t="s">
         <v>44</v>
       </c>
       <c r="T67" s="3"/>
       <c r="U67" s="3"/>
     </row>
-    <row r="68" spans="1:21" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" ht="294.5" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -5373,13 +5375,13 @@
       </c>
       <c r="M68" s="9"/>
       <c r="N68" s="3"/>
-      <c r="P68" s="18" t="s">
+      <c r="P68" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q68" s="18" t="s">
+      <c r="Q68" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R68" s="18" t="s">
+      <c r="R68" s="2" t="s">
         <v>204</v>
       </c>
       <c r="S68" s="1" t="s">
@@ -5388,7 +5390,7 @@
       <c r="T68" s="3"/>
       <c r="U68" s="3"/>
     </row>
-    <row r="69" spans="1:21" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -5423,22 +5425,22 @@
         <v>398</v>
       </c>
       <c r="N69" s="3"/>
-      <c r="P69" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q69" s="18" t="s">
+      <c r="P69" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q69" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="R69" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S69" s="18" t="s">
+      <c r="R69" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S69" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T69" s="3"/>
       <c r="U69" s="3"/>
     </row>
-    <row r="70" spans="1:21" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -5471,13 +5473,13 @@
       </c>
       <c r="M70" s="9"/>
       <c r="N70" s="3"/>
-      <c r="P70" s="18" t="s">
+      <c r="P70" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q70" s="18" t="s">
+      <c r="Q70" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R70" s="18" t="s">
+      <c r="R70" s="2" t="s">
         <v>33</v>
       </c>
       <c r="S70" s="1" t="s">
@@ -5486,7 +5488,7 @@
       <c r="T70" s="3"/>
       <c r="U70" s="3"/>
     </row>
-    <row r="71" spans="1:21" ht="51" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" ht="50" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -5517,22 +5519,22 @@
       <c r="L71" s="3"/>
       <c r="M71" s="9"/>
       <c r="N71" s="3"/>
-      <c r="P71" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q71" s="18" t="s">
+      <c r="P71" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q71" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R71" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S71" s="18" t="s">
+      <c r="R71" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S71" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T71" s="3"/>
       <c r="U71" s="3"/>
     </row>
-    <row r="72" spans="1:21" ht="51" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" ht="50" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -5563,22 +5565,22 @@
       <c r="L72" s="3"/>
       <c r="M72" s="9"/>
       <c r="N72" s="3"/>
-      <c r="P72" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q72" s="18" t="s">
+      <c r="P72" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q72" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R72" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S72" s="18" t="s">
+      <c r="R72" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S72" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T72" s="3"/>
       <c r="U72" s="3"/>
     </row>
-    <row r="73" spans="1:21" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" ht="137.5" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -5609,16 +5611,16 @@
       <c r="L73" s="3"/>
       <c r="M73" s="9"/>
       <c r="N73" s="3"/>
-      <c r="P73" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q73" s="18" t="s">
+      <c r="P73" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q73" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="R73" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S73" s="18" t="s">
+      <c r="R73" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S73" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T73" s="15" t="s">
@@ -5626,7 +5628,7 @@
       </c>
       <c r="U73" s="3"/>
     </row>
-    <row r="74" spans="1:21" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -5657,22 +5659,22 @@
       <c r="L74" s="3"/>
       <c r="M74" s="9"/>
       <c r="N74" s="3"/>
-      <c r="P74" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q74" s="18" t="s">
+      <c r="P74" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q74" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R74" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S74" s="18" t="s">
+      <c r="R74" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S74" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T74" s="3"/>
       <c r="U74" s="3"/>
     </row>
-    <row r="75" spans="1:21" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -5703,22 +5705,22 @@
       <c r="L75" s="3"/>
       <c r="M75" s="9"/>
       <c r="N75" s="3"/>
-      <c r="P75" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q75" s="18" t="s">
+      <c r="P75" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q75" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R75" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S75" s="18" t="s">
+      <c r="R75" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S75" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T75" s="3"/>
       <c r="U75" s="3"/>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -5749,22 +5751,22 @@
       <c r="L76" s="3"/>
       <c r="M76" s="9"/>
       <c r="N76" s="3"/>
-      <c r="P76" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q76" s="18" t="s">
+      <c r="P76" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q76" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R76" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S76" s="18" t="s">
+      <c r="R76" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S76" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T76" s="3"/>
       <c r="U76" s="3"/>
     </row>
-    <row r="77" spans="1:21" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" ht="75" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -5795,22 +5797,22 @@
       <c r="L77" s="3"/>
       <c r="M77" s="9"/>
       <c r="N77" s="3"/>
-      <c r="P77" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q77" s="18" t="s">
+      <c r="P77" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q77" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R77" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S77" s="18" t="s">
+      <c r="R77" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S77" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T77" s="3"/>
       <c r="U77" s="3"/>
     </row>
-    <row r="78" spans="1:21" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -5841,22 +5843,22 @@
       <c r="L78" s="3"/>
       <c r="M78" s="9"/>
       <c r="N78" s="3"/>
-      <c r="P78" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q78" s="18" t="s">
+      <c r="P78" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q78" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="R78" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S78" s="18" t="s">
+      <c r="R78" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S78" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T78" s="3"/>
       <c r="U78" s="3"/>
     </row>
-    <row r="79" spans="1:21" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -5891,22 +5893,22 @@
         <v>405</v>
       </c>
       <c r="N79" s="3"/>
-      <c r="P79" s="18" t="s">
+      <c r="P79" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q79" s="18" t="s">
+      <c r="Q79" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R79" s="18" t="s">
+      <c r="R79" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S79" s="18" t="s">
+      <c r="S79" s="2" t="s">
         <v>44</v>
       </c>
       <c r="T79" s="3"/>
       <c r="U79" s="3"/>
     </row>
-    <row r="80" spans="1:21" ht="186" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" ht="168.5" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -5944,13 +5946,13 @@
       <c r="O80" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="P80" s="18" t="s">
+      <c r="P80" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q80" s="18" t="s">
+      <c r="Q80" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R80" s="18" t="s">
+      <c r="R80" s="2" t="s">
         <v>204</v>
       </c>
       <c r="S80" s="1" t="s">
@@ -5959,7 +5961,7 @@
       <c r="T80" s="3"/>
       <c r="U80" s="3"/>
     </row>
-    <row r="81" spans="1:21" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" ht="25" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -5990,22 +5992,22 @@
       <c r="L81" s="3"/>
       <c r="M81" s="9"/>
       <c r="N81" s="3"/>
-      <c r="P81" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q81" s="18" t="s">
+      <c r="P81" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q81" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R81" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S81" s="18" t="s">
+      <c r="R81" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S81" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T81" s="3"/>
       <c r="U81" s="3"/>
     </row>
-    <row r="82" spans="1:21" ht="102" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" ht="100" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -6040,22 +6042,22 @@
         <v>411</v>
       </c>
       <c r="N82" s="3"/>
-      <c r="P82" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q82" s="18" t="s">
+      <c r="P82" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q82" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="R82" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S82" s="18" t="s">
+      <c r="R82" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S82" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T82" s="3"/>
       <c r="U82" s="3"/>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -6084,22 +6086,22 @@
       <c r="L83" s="3"/>
       <c r="M83" s="9"/>
       <c r="N83" s="3"/>
-      <c r="P83" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q83" s="18" t="s">
+      <c r="P83" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q83" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R83" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S83" s="18" t="s">
+      <c r="R83" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S83" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T83" s="3"/>
       <c r="U83" s="3"/>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -6130,16 +6132,16 @@
       <c r="L84" s="3"/>
       <c r="M84" s="9"/>
       <c r="N84" s="3"/>
-      <c r="P84" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q84" s="18" t="s">
+      <c r="P84" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q84" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="R84" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="S84" s="18" t="s">
+      <c r="R84" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S84" s="2" t="s">
         <v>59</v>
       </c>
       <c r="T84" s="3"/>

</xml_diff>

<commit_message>
correcting variable name for age to upper case
</commit_message>
<xml_diff>
--- a/data_processing_elements-CHS.xlsx
+++ b/data_processing_elements-CHS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maelstrom\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F66206E-B8AD-4495-A810-0BAA59F5F05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC856D9-B119-4842-84EA-8D292213726B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1530,10 +1530,10 @@
     <t>round(rowMeans(select(., V22_1, V22_2, V22_3), na.rm=TRUE), 2)</t>
   </si>
   <si>
-    <t>k0alder5</t>
-  </si>
-  <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>K0ALDER5</t>
   </si>
 </sst>
 </file>
@@ -2042,10 +2042,10 @@
   <dimension ref="A1:U84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomRight" activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2160,7 +2160,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="9"/>
       <c r="J2" s="12" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>290</v>
@@ -2306,7 +2306,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="9"/>
       <c r="J5" s="12" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>

</xml_diff>

<commit_message>
Correcting diabetes and Tv week all harmo rules
</commit_message>
<xml_diff>
--- a/data_processing_elements-CHS.xlsx
+++ b/data_processing_elements-CHS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maelstrom\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC856D9-B119-4842-84EA-8D292213726B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADB27F3-1361-4144-8DBF-13AF9932260B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1385,11 +1385,6 @@
     <t>do you daily or nearly daily use: diabetic medication</t>
   </si>
   <si>
-    <t>case_when(m12 == 1|
-m11 == 1;
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
     <t>Sub89</t>
   </si>
   <si>
@@ -1433,30 +1428,6 @@
 for how long do you watch television per day (minutes)</t>
   </si>
   <si>
-    <t>case_when(
-rowSums(mutate(.,
-temp_Sub86a = Sub86a,
-temp_Sub86b = Sub86b/60) %&gt;%
-select(temp_Sub86a, temp_Sub86b), 
-na.rm = TRUE) &lt;= 1 ~ 1L;
-rowSums(mutate(.,
-temp_Sub86a = Sub86a,
-temp_Sub86b = Sub86b/60) %&gt;%
-select(temp_Sub86a, temp_Sub86b), 
-na.rm = TRUE) &lt;= 1 ~ 1L; &lt;= 3 &amp; 
-rowSums(mutate(.,
-temp_Sub86a = Sub86a,
-temp_Sub86b = Sub86b/60) %&gt;%
-select(temp_Sub86a, temp_Sub86b), 
-na.rm = TRUE) &lt;= 1 ~ 1L; &gt; 1 ~ 2L;
-rowSums(mutate(.,
-temp_Sub86a = Sub86a,
-temp_Sub86b = Sub86b/60) %&gt;%
-select(temp_Sub86a, temp_Sub86b), 
-na.rm = TRUE) &lt;= 1 ~ 1L; &gt; 3 ~ 3L;
-ELSE ~ NA_integer_)</t>
-  </si>
-  <si>
     <t>Variable Sub87a appears twice in your data dictionary (probably a typo, should be Sub87b). Are these variables specific to computer use outside of work hours or not?</t>
   </si>
   <si>
@@ -1534,6 +1505,29 @@
   </si>
   <si>
     <t>K0ALDER5</t>
+  </si>
+  <si>
+    <t>case_when(
+  rowSums(mutate(.,
+                 temp_Sub86a = Sub86a,
+                 temp_Sub86b = Sub86b/60) %&gt;%
+            select(temp_Sub86a, temp_Sub86b), 
+          na.rm = TRUE) &lt;= 1 ~ 1L;
+  rowSums(mutate(.,
+                 temp_Sub86a = Sub86a,
+                 temp_Sub86b = Sub86b/60) %&gt;%
+            select(temp_Sub86a, temp_Sub86b), 
+          na.rm = TRUE) &lt;= 3 ~ 2L; 
+    rowSums(mutate(.,
+                   temp_Sub86a = Sub86a,
+                   temp_Sub86b = Sub86b/60) %&gt;%
+              select(temp_Sub86a, temp_Sub86b), 
+            na.rm = TRUE) &gt; 3 ~ 3L;
+  ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>case_when(m12 == 1| m11 == 1 ~ 1L;
+ELSE ~ NA_integer_)</t>
   </si>
 </sst>
 </file>
@@ -2042,17 +2036,17 @@
   <dimension ref="A1:U84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="M70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F69" sqref="F69"/>
+      <selection pane="bottomRight" activeCell="R70" sqref="R70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4.7265625" style="2" customWidth="1"/>
     <col min="2" max="2" width="7.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.7265625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="34.7265625" style="2" customWidth="1"/>
     <col min="4" max="4" width="27.26953125" style="2" customWidth="1"/>
     <col min="5" max="5" width="30.54296875" style="2" customWidth="1"/>
     <col min="6" max="6" width="8.453125" style="2" customWidth="1"/>
@@ -2068,7 +2062,7 @@
     <col min="16" max="16" width="12.7265625" style="2" customWidth="1"/>
     <col min="17" max="17" width="12.453125" style="2" customWidth="1"/>
     <col min="18" max="18" width="17.54296875" style="2" customWidth="1"/>
-    <col min="19" max="19" width="19.81640625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="37.36328125" style="2" customWidth="1"/>
     <col min="20" max="21" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
@@ -2160,7 +2154,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="9"/>
       <c r="J2" s="12" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>290</v>
@@ -2226,7 +2220,7 @@
         <v>33</v>
       </c>
       <c r="S3" s="18" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
@@ -2306,7 +2300,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="9"/>
       <c r="J5" s="12" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -2374,7 +2368,7 @@
         <v>39</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
@@ -2797,7 +2791,7 @@
         <v>26</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="S15" s="2">
         <v>2</v>
@@ -3313,7 +3307,7 @@
         <v>33</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
@@ -3368,7 +3362,7 @@
         <v>33</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
@@ -4197,7 +4191,7 @@
         <v>33</v>
       </c>
       <c r="S43" s="16" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="T43" s="3"/>
       <c r="U43" s="3"/>
@@ -4841,7 +4835,7 @@
       <c r="T56" s="3"/>
       <c r="U56" s="3"/>
     </row>
-    <row r="57" spans="1:21" ht="70.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:21" ht="28.5" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -4886,7 +4880,7 @@
         <v>204</v>
       </c>
       <c r="S57" s="1" t="s">
-        <v>391</v>
+        <v>419</v>
       </c>
       <c r="T57" s="3"/>
       <c r="U57" s="3"/>
@@ -5316,16 +5310,16 @@
       <c r="H67" s="3"/>
       <c r="I67" s="9"/>
       <c r="J67" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K67" s="3"/>
       <c r="L67" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="M67" s="9"/>
       <c r="N67" s="3"/>
       <c r="O67" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="P67" s="2" t="s">
         <v>25</v>
@@ -5367,11 +5361,11 @@
         <v>234</v>
       </c>
       <c r="J68" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K68" s="3"/>
       <c r="L68" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="M68" s="9"/>
       <c r="N68" s="3"/>
@@ -5385,7 +5379,7 @@
         <v>204</v>
       </c>
       <c r="S68" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="T68" s="3"/>
       <c r="U68" s="3"/>
@@ -5415,14 +5409,14 @@
         <v>237</v>
       </c>
       <c r="J69" s="12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="K69" s="3"/>
       <c r="L69" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="M69" s="9" t="s">
         <v>397</v>
-      </c>
-      <c r="M69" s="9" t="s">
-        <v>398</v>
       </c>
       <c r="N69" s="3"/>
       <c r="P69" s="2" t="s">
@@ -5440,7 +5434,7 @@
       <c r="T69" s="3"/>
       <c r="U69" s="3"/>
     </row>
-    <row r="70" spans="1:21" ht="409.6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:21" ht="322.5" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -5465,11 +5459,11 @@
         <v>240</v>
       </c>
       <c r="J70" s="12" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="K70" s="3"/>
       <c r="L70" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="M70" s="9"/>
       <c r="N70" s="3"/>
@@ -5483,7 +5477,7 @@
         <v>33</v>
       </c>
       <c r="S70" s="1" t="s">
-        <v>401</v>
+        <v>418</v>
       </c>
       <c r="T70" s="3"/>
       <c r="U70" s="3"/>
@@ -5624,7 +5618,7 @@
         <v>59</v>
       </c>
       <c r="T73" s="15" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="U73" s="3"/>
     </row>
@@ -5883,14 +5877,14 @@
         <v>270</v>
       </c>
       <c r="J79" s="12" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="K79" s="3"/>
       <c r="L79" s="3" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="M79" s="9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="N79" s="3"/>
       <c r="P79" s="2" t="s">
@@ -5933,18 +5927,18 @@
         <v>188</v>
       </c>
       <c r="J80" s="12" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="K80" s="3"/>
       <c r="L80" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="M80" s="9" t="s">
         <v>368</v>
       </c>
       <c r="N80" s="3"/>
       <c r="O80" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="P80" s="2" t="s">
         <v>25</v>
@@ -5956,7 +5950,7 @@
         <v>204</v>
       </c>
       <c r="S80" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="T80" s="3"/>
       <c r="U80" s="3"/>
@@ -6036,10 +6030,10 @@
       </c>
       <c r="K82" s="3"/>
       <c r="L82" s="3" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="M82" s="9" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="N82" s="3"/>
       <c r="P82" s="2" t="s">

</xml_diff>

<commit_message>
changing rule category for tv week all
</commit_message>
<xml_diff>
--- a/data_processing_elements-CHS.xlsx
+++ b/data_processing_elements-CHS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maelstrom\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADB27F3-1361-4144-8DBF-13AF9932260B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0393619-D475-4B7A-8064-1944047A6B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -2039,7 +2039,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="M70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R70" sqref="R70"/>
+      <selection pane="bottomRight" activeCell="Q70" sqref="Q70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2061,7 +2061,7 @@
     <col min="15" max="15" width="21.26953125" style="2" customWidth="1"/>
     <col min="16" max="16" width="12.7265625" style="2" customWidth="1"/>
     <col min="17" max="17" width="12.453125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="17.54296875" style="2" customWidth="1"/>
+    <col min="18" max="18" width="17.36328125" style="2" customWidth="1"/>
     <col min="19" max="19" width="37.36328125" style="2" customWidth="1"/>
     <col min="20" max="21" width="9.1796875" style="2"/>
   </cols>
@@ -4148,7 +4148,7 @@
       <c r="T42" s="3"/>
       <c r="U42" s="3"/>
     </row>
-    <row r="43" spans="1:21" ht="71" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:21" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>49</v>
       </c>
       <c r="R70" s="2" t="s">
-        <v>33</v>
+        <v>204</v>
       </c>
       <c r="S70" s="1" t="s">
         <v>418</v>
@@ -5902,7 +5902,7 @@
       <c r="T79" s="3"/>
       <c r="U79" s="3"/>
     </row>
-    <row r="80" spans="1:21" ht="168.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:21" ht="140" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
correct education harmo rule
</commit_message>
<xml_diff>
--- a/data_processing_elements-CHS.xlsx
+++ b/data_processing_elements-CHS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6988A27-236F-40AF-B0D6-BF83F70043F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9203C2AC-4320-4EB4-84ED-A6180A9814C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="465" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="469">
   <si>
     <t>index</t>
   </si>
@@ -1522,9 +1522,6 @@
   </si>
   <si>
     <t>Birth year: full four digits year. Birth month: number of month in the calendar, e.g. 1 for january. Birthday: date of birth, e.g. 1 the first day in the month. Examination date: datemonthyear</t>
-  </si>
-  <si>
-    <t>recode(0=0; 1=NA; 2=NA; 3=NA; 4=3; ELSE=NA)</t>
   </si>
   <si>
     <t>recoded cat 4 was not included</t>
@@ -1698,6 +1695,13 @@
   </si>
   <si>
     <t>format(as.Date(us, format = "%d/%m/%Y"), "%Y-%m-%d")</t>
+  </si>
+  <si>
+    <t>recode(0=0; 1=1; 2=1; 3=2; 4=3; ELSE=NA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The years of education are years of education post primary school, thus I would suggest to code our category of 1-3 years education as 1 in your coding and &gt;3 years education as 2 in your coding.
+</t>
   </si>
 </sst>
 </file>
@@ -1810,7 +1814,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1865,6 +1869,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2209,10 +2216,10 @@
   <dimension ref="A1:AD84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="O5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W6" sqref="W6"/>
+      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2428,7 +2435,7 @@
         <v>32</v>
       </c>
       <c r="W3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="X3" t="s">
         <v>419</v>
@@ -2543,7 +2550,7 @@
         <v>32</v>
       </c>
       <c r="W5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="Y5" t="s">
         <v>426</v>
@@ -2552,7 +2559,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="171.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2603,19 +2610,22 @@
         <v>38</v>
       </c>
       <c r="W6" t="s">
+        <v>467</v>
+      </c>
+      <c r="X6" t="s">
         <v>428</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>429</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="AA6" t="s">
         <v>430</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>431</v>
       </c>
-      <c r="AB6" t="s">
-        <v>432</v>
+      <c r="AC6" s="22" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="171.75" x14ac:dyDescent="0.25">
@@ -2670,16 +2680,16 @@
         <v>58</v>
       </c>
       <c r="X7" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="Y7" t="s">
         <v>300</v>
       </c>
       <c r="AA7" t="s">
+        <v>433</v>
+      </c>
+      <c r="AB7" t="s">
         <v>434</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="8" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
@@ -2726,16 +2736,16 @@
         <v>58</v>
       </c>
       <c r="X8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="Y8" t="s">
         <v>301</v>
       </c>
       <c r="AA8" t="s">
+        <v>436</v>
+      </c>
+      <c r="AB8" t="s">
         <v>437</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="9" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
@@ -2866,13 +2876,13 @@
         <v>58</v>
       </c>
       <c r="X11" s="21" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Y11" s="21" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="12" spans="1:30" ht="345" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2916,7 +2926,7 @@
         <v>58</v>
       </c>
       <c r="X12" s="21" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="13" spans="1:30" ht="114.75" x14ac:dyDescent="0.25">
@@ -2970,7 +2980,7 @@
         <v>58</v>
       </c>
       <c r="X13" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="14" spans="1:30" ht="114.75" x14ac:dyDescent="0.25">
@@ -3071,10 +3081,10 @@
         <v>307</v>
       </c>
       <c r="AA15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="AB15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -3188,10 +3198,10 @@
         <v>312</v>
       </c>
       <c r="AA17" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="AB17" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
@@ -3305,10 +3315,10 @@
         <v>312</v>
       </c>
       <c r="AA19" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="AB19" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
@@ -3813,7 +3823,7 @@
         <v>331</v>
       </c>
       <c r="X29" s="21" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
@@ -3868,10 +3878,10 @@
         <v>334</v>
       </c>
       <c r="AA30" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="AB30" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
@@ -4022,16 +4032,16 @@
         <v>43</v>
       </c>
       <c r="X33" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="Y33" t="s">
         <v>340</v>
       </c>
       <c r="AA33" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="AB33" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.25">
@@ -4342,7 +4352,7 @@
         <v>354</v>
       </c>
       <c r="X39" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
@@ -4441,7 +4451,7 @@
         <v>354</v>
       </c>
       <c r="X41" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="42" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4516,7 +4526,7 @@
         <v>357</v>
       </c>
       <c r="K43" s="12" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="L43" s="3"/>
       <c r="M43" s="9"/>
@@ -4525,11 +4535,11 @@
         <v>418</v>
       </c>
       <c r="Q43" s="16" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="R43" s="16"/>
       <c r="S43" s="16" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="T43" s="3" t="s">
         <v>24</v>
@@ -4541,16 +4551,16 @@
         <v>32</v>
       </c>
       <c r="W43" t="s">
+        <v>450</v>
+      </c>
+      <c r="X43" t="s">
         <v>451</v>
       </c>
-      <c r="X43" t="s">
+      <c r="Y43" s="21" t="s">
         <v>452</v>
       </c>
-      <c r="Y43" s="21" t="s">
+      <c r="AA43" t="s">
         <v>453</v>
-      </c>
-      <c r="AA43" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="44" spans="1:28" ht="225" x14ac:dyDescent="0.25">
@@ -4575,13 +4585,13 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="J44" s="12" t="s">
         <v>358</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="L44" s="3"/>
       <c r="M44" s="9" t="s">
@@ -4683,7 +4693,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="J46" s="12" t="s">
         <v>362</v>
@@ -4902,7 +4912,7 @@
         <v>364</v>
       </c>
       <c r="S50" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="T50" s="3" t="s">
         <v>24</v>
@@ -5268,7 +5278,7 @@
         <v>201</v>
       </c>
       <c r="W57" s="21" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="58" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
@@ -5752,7 +5762,7 @@
         <v>201</v>
       </c>
       <c r="W68" s="21" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="69" spans="1:28" ht="200.25" x14ac:dyDescent="0.25">
@@ -5854,10 +5864,10 @@
         <v>201</v>
       </c>
       <c r="W70" s="21" t="s">
+        <v>459</v>
+      </c>
+      <c r="X70" t="s">
         <v>460</v>
-      </c>
-      <c r="X70" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="71" spans="1:28" ht="51" x14ac:dyDescent="0.25">
@@ -5995,10 +6005,10 @@
         <v>395</v>
       </c>
       <c r="AA73" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="AB73" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="74" spans="1:28" ht="38.25" x14ac:dyDescent="0.25">
@@ -6328,7 +6338,7 @@
         <v>402</v>
       </c>
       <c r="X80" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="81" spans="1:26" ht="25.5" x14ac:dyDescent="0.25">
@@ -6427,10 +6437,10 @@
         <v>58</v>
       </c>
       <c r="X82" t="s">
+        <v>463</v>
+      </c>
+      <c r="Z82" s="21" t="s">
         <v>464</v>
-      </c>
-      <c r="Z82" s="21" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
correct id variable name
</commit_message>
<xml_diff>
--- a/data_processing_elements-CHS.xlsx
+++ b/data_processing_elements-CHS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9203C2AC-4320-4EB4-84ED-A6180A9814C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF67B7B-8AA7-4B1E-AB33-ED96948ACB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="465" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements" sheetId="8" r:id="rId1"/>
@@ -962,9 +962,6 @@
     <t>CHS</t>
   </si>
   <si>
-    <t>Id</t>
-  </si>
-  <si>
     <t>Id number in CCHS5</t>
   </si>
   <si>
@@ -1702,6 +1699,9 @@
   <si>
     <t xml:space="preserve">The years of education are years of education post primary school, thus I would suggest to code our category of 1-3 years education as 1 in your coding and &gt;3 years education as 2 in your coding.
 </t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -1814,7 +1814,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1871,9 +1871,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1897,7 +1894,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2216,13 +2213,13 @@
   <dimension ref="A1:AD84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="O5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
+      <selection pane="bottomRight" activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" style="2" customWidth="1"/>
@@ -2240,13 +2237,15 @@
     <col min="14" max="14" width="7.7109375" style="2" customWidth="1"/>
     <col min="15" max="15" width="21.28515625" style="2" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="36.5703125" style="2" customWidth="1"/>
     <col min="18" max="18" width="17.42578125" style="2" customWidth="1"/>
     <col min="19" max="19" width="37.42578125" style="2" customWidth="1"/>
-    <col min="20" max="21" width="9.140625" style="2"/>
+    <col min="20" max="20" width="11.7109375" style="2" customWidth="1"/>
+    <col min="21" max="21" width="13.140625" style="2" customWidth="1"/>
     <col min="22" max="22" width="29.140625" customWidth="1"/>
-    <col min="23" max="23" width="26.7109375" customWidth="1"/>
+    <col min="23" max="23" width="81.42578125" customWidth="1"/>
     <col min="24" max="24" width="26.28515625" customWidth="1"/>
+    <col min="29" max="29" width="55.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
@@ -2284,19 +2283,19 @@
         <v>10</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M1" s="13" t="s">
         <v>11</v>
       </c>
       <c r="N1" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>409</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="17" t="s">
         <v>410</v>
-      </c>
-      <c r="P1" s="17" t="s">
-        <v>411</v>
       </c>
       <c r="Q1" s="17" t="s">
         <v>12</v>
@@ -2320,25 +2319,25 @@
         <v>18</v>
       </c>
       <c r="X1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Y1" t="s">
         <v>19</v>
       </c>
       <c r="Z1" t="s">
+        <v>412</v>
+      </c>
+      <c r="AA1" t="s">
         <v>413</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>414</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>415</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>416</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
@@ -2364,16 +2363,16 @@
       <c r="H2" s="3"/>
       <c r="I2" s="9"/>
       <c r="J2" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>286</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>287</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="9"/>
       <c r="N2" s="3"/>
       <c r="P2" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>24</v>
@@ -2385,7 +2384,7 @@
         <v>26</v>
       </c>
       <c r="W2" t="s">
-        <v>286</v>
+        <v>468</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
@@ -2413,16 +2412,16 @@
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>288</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>289</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="9"/>
       <c r="N3" s="3"/>
       <c r="P3" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="S3" s="18"/>
       <c r="T3" s="3" t="s">
@@ -2435,19 +2434,19 @@
         <v>32</v>
       </c>
       <c r="W3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="X3" t="s">
+        <v>418</v>
+      </c>
+      <c r="Y3" t="s">
         <v>419</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AA3" t="s">
         <v>420</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>421</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="30" thickBot="1" x14ac:dyDescent="0.3">
@@ -2475,7 +2474,7 @@
         <v>37</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>34</v>
@@ -2484,10 +2483,10 @@
       <c r="M4" s="9"/>
       <c r="N4" s="3"/>
       <c r="P4" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="T4" s="3" t="s">
         <v>24</v>
@@ -2499,7 +2498,7 @@
         <v>38</v>
       </c>
       <c r="W4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2527,16 +2526,16 @@
       <c r="H5" s="3"/>
       <c r="I5" s="9"/>
       <c r="J5" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="K5" s="12" t="s">
         <v>424</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>425</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="9"/>
       <c r="N5" s="3"/>
       <c r="P5" s="19" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R5" s="20"/>
       <c r="S5" s="20"/>
@@ -2550,16 +2549,16 @@
         <v>32</v>
       </c>
       <c r="W5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="Y5" t="s">
+        <v>425</v>
+      </c>
+      <c r="AA5" t="s">
         <v>426</v>
       </c>
-      <c r="AA5" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" ht="409.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:30" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2584,21 +2583,21 @@
         <v>47</v>
       </c>
       <c r="J6" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>293</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>294</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N6" s="3"/>
       <c r="P6" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="T6" s="3" t="s">
         <v>24</v>
@@ -2610,25 +2609,25 @@
         <v>38</v>
       </c>
       <c r="W6" t="s">
+        <v>466</v>
+      </c>
+      <c r="X6" t="s">
+        <v>427</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>428</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>429</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>430</v>
+      </c>
+      <c r="AC6" s="21" t="s">
         <v>467</v>
       </c>
-      <c r="X6" t="s">
-        <v>428</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>429</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>430</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>431</v>
-      </c>
-      <c r="AC6" s="22" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" ht="171.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:30" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2653,19 +2652,19 @@
         <v>52</v>
       </c>
       <c r="J7" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>297</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>298</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="9"/>
       <c r="N7" s="3"/>
       <c r="P7" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="T7" s="15" t="s">
         <v>58</v>
@@ -2680,16 +2679,16 @@
         <v>58</v>
       </c>
       <c r="X7" t="s">
+        <v>431</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>299</v>
+      </c>
+      <c r="AA7" t="s">
         <v>432</v>
       </c>
-      <c r="Y7" t="s">
-        <v>300</v>
-      </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>433</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="8" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
@@ -2736,16 +2735,16 @@
         <v>58</v>
       </c>
       <c r="X8" t="s">
+        <v>434</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>300</v>
+      </c>
+      <c r="AA8" t="s">
         <v>435</v>
       </c>
-      <c r="Y8" t="s">
-        <v>301</v>
-      </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>436</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="9" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
@@ -2834,7 +2833,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2876,10 +2875,10 @@
         <v>58</v>
       </c>
       <c r="X11" s="21" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="Y11" s="21" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="12" spans="1:30" ht="135" x14ac:dyDescent="0.25">
@@ -2926,10 +2925,10 @@
         <v>58</v>
       </c>
       <c r="X12" s="21" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" ht="114.75" x14ac:dyDescent="0.25">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2954,18 +2953,18 @@
         <v>78</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>305</v>
       </c>
       <c r="T13" s="3" t="s">
         <v>58</v>
@@ -2980,10 +2979,10 @@
         <v>58</v>
       </c>
       <c r="X13" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" ht="114.75" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -3008,18 +3007,18 @@
         <v>82</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="Q14" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>305</v>
       </c>
       <c r="T14" s="3" t="s">
         <v>24</v>
@@ -3031,7 +3030,7 @@
         <v>38</v>
       </c>
       <c r="W14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="15" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
@@ -3072,19 +3071,19 @@
         <v>25</v>
       </c>
       <c r="V15" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="W15">
         <v>2</v>
       </c>
       <c r="Y15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AA15" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="AB15" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -3112,18 +3111,18 @@
       <c r="H16" s="3"/>
       <c r="I16" s="9"/>
       <c r="J16" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="K16" s="3" t="s">
         <v>308</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>309</v>
       </c>
       <c r="L16" s="3"/>
       <c r="M16" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N16" s="3"/>
       <c r="P16" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R16" s="2" t="s">
         <v>88</v>
@@ -3166,18 +3165,18 @@
         <v>91</v>
       </c>
       <c r="J17" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="K17" s="3" t="s">
         <v>308</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>309</v>
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N17" s="3"/>
       <c r="P17" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R17" s="2" t="s">
         <v>88</v>
@@ -3192,16 +3191,16 @@
         <v>32</v>
       </c>
       <c r="W17" t="s">
+        <v>310</v>
+      </c>
+      <c r="Y17" t="s">
         <v>311</v>
       </c>
-      <c r="Y17" t="s">
-        <v>312</v>
-      </c>
       <c r="AA17" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="AB17" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
@@ -3229,18 +3228,18 @@
       <c r="H18" s="3"/>
       <c r="I18" s="9"/>
       <c r="J18" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="K18" s="3" t="s">
         <v>313</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>314</v>
       </c>
       <c r="L18" s="3"/>
       <c r="M18" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N18" s="3"/>
       <c r="P18" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R18" s="2" t="s">
         <v>94</v>
@@ -3283,18 +3282,18 @@
         <v>91</v>
       </c>
       <c r="J19" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="K19" s="3" t="s">
         <v>313</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>314</v>
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N19" s="3"/>
       <c r="P19" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R19" s="2" t="s">
         <v>94</v>
@@ -3309,16 +3308,16 @@
         <v>32</v>
       </c>
       <c r="W19" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Y19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AA19" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="AB19" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
@@ -3346,16 +3345,16 @@
       <c r="H20" s="3"/>
       <c r="I20" s="9"/>
       <c r="J20" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="K20" s="3" t="s">
         <v>317</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>318</v>
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="9"/>
       <c r="N20" s="3"/>
       <c r="P20" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R20" s="2" t="s">
         <v>99</v>
@@ -3398,18 +3397,18 @@
       <c r="H21" s="3"/>
       <c r="I21" s="9"/>
       <c r="J21" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="K21" s="3" t="s">
         <v>319</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>320</v>
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="N21" s="3"/>
       <c r="P21" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R21" s="2" t="s">
         <v>88</v>
@@ -3452,18 +3451,18 @@
         <v>91</v>
       </c>
       <c r="J22" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="K22" s="3" t="s">
         <v>319</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>320</v>
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="N22" s="3"/>
       <c r="P22" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R22" s="2" t="s">
         <v>88</v>
@@ -3478,7 +3477,7 @@
         <v>32</v>
       </c>
       <c r="W22" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
@@ -3592,18 +3591,18 @@
       <c r="H25" s="3"/>
       <c r="I25" s="9"/>
       <c r="J25" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="K25" s="3" t="s">
         <v>323</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>324</v>
       </c>
       <c r="L25" s="3"/>
       <c r="M25" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N25" s="3"/>
       <c r="P25" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R25" s="2" t="s">
         <v>113</v>
@@ -3621,7 +3620,7 @@
         <v>32</v>
       </c>
       <c r="W25" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="26" spans="1:28" ht="42.75" x14ac:dyDescent="0.25">
@@ -3649,18 +3648,18 @@
       <c r="H26" s="3"/>
       <c r="I26" s="9"/>
       <c r="J26" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="K26" s="3" t="s">
         <v>325</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>326</v>
       </c>
       <c r="L26" s="3"/>
       <c r="M26" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N26" s="3"/>
       <c r="P26" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R26" s="2" t="s">
         <v>113</v>
@@ -3678,7 +3677,7 @@
         <v>32</v>
       </c>
       <c r="W26" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
@@ -3769,7 +3768,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="228.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" ht="129" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -3794,21 +3793,21 @@
         <v>125</v>
       </c>
       <c r="J29" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="K29" s="3" t="s">
         <v>327</v>
-      </c>
-      <c r="K29" s="3" t="s">
-        <v>328</v>
       </c>
       <c r="L29" s="3"/>
       <c r="M29" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="N29" s="3"/>
       <c r="P29" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="T29" s="3" t="s">
         <v>24</v>
@@ -3820,10 +3819,10 @@
         <v>38</v>
       </c>
       <c r="W29" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="X29" s="21" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
@@ -3851,16 +3850,16 @@
       <c r="H30" s="3"/>
       <c r="I30" s="9"/>
       <c r="J30" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="K30" s="3" t="s">
         <v>332</v>
-      </c>
-      <c r="K30" s="3" t="s">
-        <v>333</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="9"/>
       <c r="N30" s="3"/>
       <c r="P30" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="T30" s="15" t="s">
         <v>24</v>
@@ -3875,13 +3874,13 @@
         <v>43</v>
       </c>
       <c r="Y30" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AA30" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AB30" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
@@ -3953,19 +3952,19 @@
       <c r="H32" s="3"/>
       <c r="I32" s="9"/>
       <c r="J32" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="K32" s="3" t="s">
         <v>335</v>
-      </c>
-      <c r="K32" s="3" t="s">
-        <v>336</v>
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="9"/>
       <c r="N32" s="3"/>
       <c r="P32" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="T32" s="3" t="s">
         <v>24</v>
@@ -4005,19 +4004,19 @@
       <c r="H33" s="3"/>
       <c r="I33" s="9"/>
       <c r="J33" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="K33" s="3" t="s">
         <v>338</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>339</v>
       </c>
       <c r="L33" s="3"/>
       <c r="M33" s="9"/>
       <c r="N33" s="3"/>
       <c r="P33" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="T33" s="15" t="s">
         <v>24</v>
@@ -4032,16 +4031,16 @@
         <v>43</v>
       </c>
       <c r="X33" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="Y33" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AA33" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="AB33" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.25">
@@ -4069,19 +4068,19 @@
       <c r="H34" s="3"/>
       <c r="I34" s="9"/>
       <c r="J34" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="K34" s="3" t="s">
         <v>341</v>
-      </c>
-      <c r="K34" s="3" t="s">
-        <v>342</v>
       </c>
       <c r="L34" s="3"/>
       <c r="M34" s="9"/>
       <c r="N34" s="3"/>
       <c r="P34" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="T34" s="3" t="s">
         <v>24</v>
@@ -4121,20 +4120,20 @@
       <c r="H35" s="3"/>
       <c r="I35" s="9"/>
       <c r="J35" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="K35" s="12" t="s">
         <v>343</v>
-      </c>
-      <c r="K35" s="12" t="s">
-        <v>344</v>
       </c>
       <c r="L35" s="3"/>
       <c r="M35" s="9"/>
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
       <c r="P35" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="S35" s="2" t="s">
         <v>284</v>
@@ -4149,7 +4148,7 @@
         <v>32</v>
       </c>
       <c r="W35" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.25">
@@ -4177,19 +4176,19 @@
       <c r="H36" s="3"/>
       <c r="I36" s="9"/>
       <c r="J36" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="K36" s="3" t="s">
         <v>346</v>
-      </c>
-      <c r="K36" s="3" t="s">
-        <v>347</v>
       </c>
       <c r="L36" s="3"/>
       <c r="M36" s="9"/>
       <c r="N36" s="3"/>
       <c r="P36" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="T36" s="3" t="s">
         <v>24</v>
@@ -4229,19 +4228,19 @@
       <c r="H37" s="3"/>
       <c r="I37" s="9"/>
       <c r="J37" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="K37" s="3" t="s">
         <v>348</v>
-      </c>
-      <c r="K37" s="3" t="s">
-        <v>349</v>
       </c>
       <c r="L37" s="3"/>
       <c r="M37" s="9"/>
       <c r="N37" s="3"/>
       <c r="P37" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="T37" s="3" t="s">
         <v>24</v>
@@ -4300,7 +4299,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:28" ht="228.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -4325,19 +4324,19 @@
         <v>154</v>
       </c>
       <c r="J39" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="K39" s="3" t="s">
         <v>351</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>352</v>
       </c>
       <c r="L39" s="3"/>
       <c r="M39" s="9"/>
       <c r="N39" s="3"/>
       <c r="P39" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="T39" s="3" t="s">
         <v>24</v>
@@ -4349,10 +4348,10 @@
         <v>38</v>
       </c>
       <c r="W39" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="X39" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
@@ -4399,7 +4398,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="228.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -4424,19 +4423,19 @@
         <v>154</v>
       </c>
       <c r="J41" s="12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="N41" s="3"/>
       <c r="P41" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="T41" s="3" t="s">
         <v>24</v>
@@ -4448,10 +4447,10 @@
         <v>38</v>
       </c>
       <c r="W41" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="X41" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="42" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4523,23 +4522,23 @@
       <c r="H43" s="3"/>
       <c r="I43" s="9"/>
       <c r="J43" s="12" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K43" s="12" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="L43" s="3"/>
       <c r="M43" s="9"/>
       <c r="N43" s="3"/>
       <c r="P43" s="16" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="Q43" s="16" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="R43" s="16"/>
       <c r="S43" s="16" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="T43" s="3" t="s">
         <v>24</v>
@@ -4551,19 +4550,19 @@
         <v>32</v>
       </c>
       <c r="W43" t="s">
+        <v>449</v>
+      </c>
+      <c r="X43" t="s">
         <v>450</v>
       </c>
-      <c r="X43" t="s">
+      <c r="Y43" s="21" t="s">
         <v>451</v>
       </c>
-      <c r="Y43" s="21" t="s">
+      <c r="AA43" t="s">
         <v>452</v>
       </c>
-      <c r="AA43" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="44" spans="1:28" ht="225" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:28" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -4585,24 +4584,24 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J44" s="12" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="L44" s="3"/>
       <c r="M44" s="9" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="N44" s="3"/>
       <c r="P44" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="S44" s="1"/>
       <c r="T44" s="3" t="s">
@@ -4615,10 +4614,10 @@
         <v>201</v>
       </c>
       <c r="W44" s="21" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="45" spans="1:28" ht="105" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -4643,19 +4642,19 @@
         <v>173</v>
       </c>
       <c r="J45" s="12" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
       <c r="M45" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="N45" s="3"/>
       <c r="P45" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="S45" s="1"/>
       <c r="T45" s="3" t="s">
@@ -4668,7 +4667,7 @@
         <v>201</v>
       </c>
       <c r="W45" s="21" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="46" spans="1:28" ht="29.25" x14ac:dyDescent="0.25">
@@ -4693,23 +4692,23 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="J46" s="12" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
       <c r="M46" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
       <c r="P46" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="T46" s="2" t="s">
         <v>58</v>
@@ -4749,16 +4748,16 @@
       <c r="H47" s="3"/>
       <c r="I47" s="9"/>
       <c r="J47" s="12" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
       <c r="M47" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="N47" s="3"/>
       <c r="P47" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="T47" s="3" t="s">
         <v>24</v>
@@ -4770,7 +4769,7 @@
         <v>32</v>
       </c>
       <c r="W47" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="48" spans="1:28" ht="51" x14ac:dyDescent="0.25">
@@ -4842,22 +4841,22 @@
         <v>185</v>
       </c>
       <c r="J49" s="12" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
       <c r="M49" s="9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="N49" s="3"/>
       <c r="P49" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="S49" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="T49" s="3" t="s">
         <v>24</v>
@@ -4869,7 +4868,7 @@
         <v>201</v>
       </c>
       <c r="W49" s="21" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="50" spans="1:23" ht="45" x14ac:dyDescent="0.25">
@@ -4897,22 +4896,22 @@
         <v>185</v>
       </c>
       <c r="J50" s="12" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
       <c r="M50" s="9" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="N50" s="3"/>
       <c r="P50" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="S50" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="T50" s="3" t="s">
         <v>24</v>
@@ -4924,7 +4923,7 @@
         <v>201</v>
       </c>
       <c r="W50" s="21" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="51" spans="1:23" ht="29.25" x14ac:dyDescent="0.25">
@@ -4952,23 +4951,23 @@
         <v>185</v>
       </c>
       <c r="J51" s="12" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
       <c r="M51" s="9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
       <c r="P51" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="S51" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="T51" s="3" t="s">
         <v>24</v>
@@ -5052,19 +5051,19 @@
         <v>185</v>
       </c>
       <c r="J53" s="12" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
       <c r="M53" s="9" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="N53" s="3"/>
       <c r="P53" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="T53" s="3" t="s">
         <v>24</v>
@@ -5148,19 +5147,19 @@
         <v>185</v>
       </c>
       <c r="J55" s="12" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
       <c r="M55" s="9" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="N55" s="3"/>
       <c r="P55" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="T55" s="3" t="s">
         <v>24</v>
@@ -5200,19 +5199,19 @@
         <v>185</v>
       </c>
       <c r="J56" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
       <c r="M56" s="9" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="N56" s="3"/>
       <c r="P56" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="S56" s="1"/>
       <c r="T56" s="3" t="s">
@@ -5225,7 +5224,7 @@
         <v>201</v>
       </c>
       <c r="W56" s="21" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="57" spans="1:23" ht="60" x14ac:dyDescent="0.25">
@@ -5253,19 +5252,19 @@
         <v>185</v>
       </c>
       <c r="J57" s="12" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
       <c r="M57" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="N57" s="3"/>
       <c r="P57" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="S57" s="1"/>
       <c r="T57" s="3" t="s">
@@ -5278,7 +5277,7 @@
         <v>201</v>
       </c>
       <c r="W57" s="21" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="58" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
@@ -5688,19 +5687,19 @@
       <c r="H67" s="3"/>
       <c r="I67" s="9"/>
       <c r="J67" s="12" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
       <c r="M67" s="9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="N67" s="3"/>
       <c r="P67" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="S67" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="T67" s="3" t="s">
         <v>24</v>
@@ -5715,7 +5714,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="68" spans="1:28" ht="285" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" ht="165" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -5740,16 +5739,16 @@
         <v>231</v>
       </c>
       <c r="J68" s="12" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
       <c r="M68" s="9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="N68" s="3"/>
       <c r="P68" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="S68" s="1"/>
       <c r="T68" s="3" t="s">
@@ -5762,10 +5761,10 @@
         <v>201</v>
       </c>
       <c r="W68" s="21" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="69" spans="1:28" ht="200.25" x14ac:dyDescent="0.25">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="69" spans="1:28" ht="72" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -5790,19 +5789,19 @@
         <v>234</v>
       </c>
       <c r="J69" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
       <c r="M69" s="9" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="N69" s="3"/>
       <c r="P69" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="T69" s="3" t="s">
         <v>58</v>
@@ -5817,7 +5816,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:28" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28" ht="375" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -5842,16 +5841,16 @@
         <v>237</v>
       </c>
       <c r="J70" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
       <c r="M70" s="9" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="N70" s="3"/>
       <c r="P70" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="S70" s="1"/>
       <c r="T70" s="3" t="s">
@@ -5864,10 +5863,10 @@
         <v>201</v>
       </c>
       <c r="W70" s="21" t="s">
+        <v>458</v>
+      </c>
+      <c r="X70" t="s">
         <v>459</v>
-      </c>
-      <c r="X70" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="71" spans="1:28" ht="51" x14ac:dyDescent="0.25">
@@ -6002,13 +6001,13 @@
         <v>58</v>
       </c>
       <c r="Y73" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AA73" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="AB73" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="74" spans="1:28" ht="38.25" x14ac:dyDescent="0.25">
@@ -6231,7 +6230,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="171.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:28" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -6256,19 +6255,19 @@
         <v>267</v>
       </c>
       <c r="J79" s="12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
       <c r="M79" s="9" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="N79" s="3"/>
       <c r="P79" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q79" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="T79" s="3" t="s">
         <v>24</v>
@@ -6308,22 +6307,22 @@
         <v>185</v>
       </c>
       <c r="J80" s="12" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
       <c r="M80" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="N80" s="3"/>
       <c r="P80" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q80" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="S80" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="T80" s="3" t="s">
         <v>24</v>
@@ -6335,10 +6334,10 @@
         <v>201</v>
       </c>
       <c r="W80" s="21" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="X80" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="81" spans="1:26" ht="25.5" x14ac:dyDescent="0.25">
@@ -6385,7 +6384,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="82" spans="1:26" ht="357" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" ht="315" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -6415,14 +6414,14 @@
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
       <c r="M82" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="N82" s="3"/>
       <c r="P82" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q82" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="T82" s="3" t="s">
         <v>58</v>
@@ -6437,10 +6436,10 @@
         <v>58</v>
       </c>
       <c r="X82" t="s">
+        <v>462</v>
+      </c>
+      <c r="Z82" s="21" t="s">
         <v>463</v>
-      </c>
-      <c r="Z82" s="21" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
correct age, med_diabetes, and TV all
</commit_message>
<xml_diff>
--- a/data_processing_elements-CHS.xlsx
+++ b/data_processing_elements-CHS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF67B7B-8AA7-4B1E-AB33-ED96948ACB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB71A65-102C-41BF-8E4A-6CF99D76A569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="468">
   <si>
     <t>index</t>
   </si>
@@ -1503,18 +1503,6 @@
     <t>categorical</t>
   </si>
   <si>
-    <t>Faar;
-Fmd;
-Fdag;
-us</t>
-  </si>
-  <si>
-    <t>birth year;
-birth month;
-birth day;
-examination date</t>
-  </si>
-  <si>
     <t>Please confirm the completion date format</t>
   </si>
   <si>
@@ -1623,12 +1611,6 @@
   </si>
   <si>
     <t>osteoporosis</t>
-  </si>
-  <si>
-    <t>case_when(
-m12 == 1|
-m11 == 1;
-ELSE ~ NA_integer_)</t>
   </si>
   <si>
     <t>case_when( 
@@ -1644,64 +1626,69 @@
 ELSE ~ NA_integer_)</t>
   </si>
   <si>
+    <t>check when both input value = na</t>
+  </si>
+  <si>
+    <t>computer time use are not specified to weekdays nor domain, thus it is all use of computers participants are asked to report. One reason for the double vaiable could be that the participants are asked to report time use in hours and minutes</t>
+  </si>
+  <si>
+    <t>not an exhaustive list of sports, can't say no, or do we say no with a comment?</t>
+  </si>
+  <si>
+    <t>inactive includes physical activity less than 2 hours/week (Sub91), do we still populate and leave a comment, but 2 hours/week i a lot to be coded as no PA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">or 1=NA?
+questionnaire also has:
+2 = Light physical activity from 2 - 4 hours per week
+e.g. walks, bike rides, light gardening, light exercise gymnastics
+</t>
+  </si>
+  <si>
+    <t>format(as.Date(us, format = "%d/%m/%Y"), "%Y-%m-%d")</t>
+  </si>
+  <si>
+    <t>recode(0=0; 1=1; 2=1; 3=2; 4=3; ELSE=NA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The years of education are years of education post primary school, thus I would suggest to code our category of 1-3 years education as 1 in your coding and &gt;3 years education as 2 in your coding.
+</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>K0ALDER5</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
     <t>case_when(
 is.na(Sub86a) &amp; is.na(Sub86b) ~ NA_integer_;
 rowSums(mutate(.,
 temp_Sub86a = Sub86a,
 temp_Sub86b = Sub86b/60) %&gt;%
-select(temp_Sub86a, temp_Sub86b), 
-na.rm = TRUE) &lt;= 1 ~ 1L;
+select(temp_Sub86a, temp_Sub86b), na.rm = TRUE) &lt;= 1 ~ 1L;
 rowSums(mutate(.,
 temp_Sub86a = Sub86a,
 temp_Sub86b = Sub86b/60) %&gt;%
-select(temp_Sub86a, temp_Sub86b), 
-na.rm = TRUE) &lt;= 1 ~ 1L; &lt;= 3 &amp; 
+select(temp_Sub86a, temp_Sub86b), na.rm = TRUE)  &lt;= 3 &amp; 
 rowSums(mutate(.,
 temp_Sub86a = Sub86a,
 temp_Sub86b = Sub86b/60) %&gt;%
-select(temp_Sub86a, temp_Sub86b), 
-na.rm = TRUE) &lt;= 1 ~ 1L; &gt; 1 ~ 2L;
+select(temp_Sub86a, temp_Sub86b), na.rm = TRUE) &gt; 1 ~ 2L;
 rowSums(mutate(.,
 temp_Sub86a = Sub86a,
 temp_Sub86b = Sub86b/60) %&gt;%
-select(temp_Sub86a, temp_Sub86b), 
-na.rm = TRUE) &lt;= 1 ~ 1L; &gt; 3 ~ 3L;
+select(temp_Sub86a, temp_Sub86b), na.rm = TRUE) &gt; 3 ~ 3L;
 ELSE ~ NA_integer_)</t>
   </si>
   <si>
-    <t>check when both input value = na</t>
-  </si>
-  <si>
-    <t>computer time use are not specified to weekdays nor domain, thus it is all use of computers participants are asked to report. One reason for the double vaiable could be that the participants are asked to report time use in hours and minutes</t>
-  </si>
-  <si>
-    <t>not an exhaustive list of sports, can't say no, or do we say no with a comment?</t>
-  </si>
-  <si>
-    <t>inactive includes physical activity less than 2 hours/week (Sub91), do we still populate and leave a comment, but 2 hours/week i a lot to be coded as no PA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">or 1=NA?
-questionnaire also has:
-2 = Light physical activity from 2 - 4 hours per week
-e.g. walks, bike rides, light gardening, light exercise gymnastics
-</t>
-  </si>
-  <si>
-    <t>floor(as.numeric(difftime(format(as.Date(us, format = "%d/%m/%Y"), "%Y-%m-%d"), as.Date(paste0(Faar, "-", Fmd, "-", Fdag), format = "%Y-%m-%d"), units = "days"))/365.25)</t>
-  </si>
-  <si>
-    <t>format(as.Date(us, format = "%d/%m/%Y"), "%Y-%m-%d")</t>
-  </si>
-  <si>
-    <t>recode(0=0; 1=1; 2=1; 3=2; 4=3; ELSE=NA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The years of education are years of education post primary school, thus I would suggest to code our category of 1-3 years education as 1 in your coding and &gt;3 years education as 2 in your coding.
-</t>
-  </si>
-  <si>
-    <t>id</t>
+    <t>case_when(
+m12 == 1|m11 == 1 ~ 1L;
+m12 == 0 &amp;m11 == 0 ~ 0L;
+ELSE ~ NA_integer_)</t>
   </si>
 </sst>
 </file>
@@ -2213,10 +2200,10 @@
   <dimension ref="A1:AD84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="O49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S6" sqref="S6"/>
+      <selection pane="bottomRight" activeCell="W60" sqref="W60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2363,7 +2350,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="9"/>
       <c r="J2" s="12" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>286</v>
@@ -2384,7 +2371,7 @@
         <v>26</v>
       </c>
       <c r="W2" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
@@ -2434,7 +2421,7 @@
         <v>32</v>
       </c>
       <c r="W3" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="X3" t="s">
         <v>418</v>
@@ -2501,7 +2488,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2526,16 +2513,16 @@
       <c r="H5" s="3"/>
       <c r="I5" s="9"/>
       <c r="J5" s="12" t="s">
-        <v>423</v>
+        <v>464</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>424</v>
+        <v>465</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="9"/>
       <c r="N5" s="3"/>
       <c r="P5" s="19" t="s">
-        <v>417</v>
+        <v>36</v>
       </c>
       <c r="R5" s="20"/>
       <c r="S5" s="20"/>
@@ -2543,19 +2530,19 @@
         <v>24</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="V5" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="W5" t="s">
-        <v>464</v>
+        <v>43</v>
       </c>
       <c r="Y5" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="AA5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="140.25" x14ac:dyDescent="0.25">
@@ -2609,22 +2596,22 @@
         <v>38</v>
       </c>
       <c r="W6" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="X6" t="s">
+        <v>425</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>426</v>
+      </c>
+      <c r="AA6" t="s">
         <v>427</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="AB6" t="s">
         <v>428</v>
       </c>
-      <c r="AA6" t="s">
-        <v>429</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>430</v>
-      </c>
       <c r="AC6" s="21" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="127.5" x14ac:dyDescent="0.25">
@@ -2679,16 +2666,16 @@
         <v>58</v>
       </c>
       <c r="X7" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="Y7" t="s">
         <v>299</v>
       </c>
       <c r="AA7" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="AB7" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="8" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
@@ -2735,16 +2722,16 @@
         <v>58</v>
       </c>
       <c r="X8" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="Y8" t="s">
         <v>300</v>
       </c>
       <c r="AA8" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="AB8" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="9" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
@@ -2875,7 +2862,7 @@
         <v>58</v>
       </c>
       <c r="X11" s="21" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="Y11" s="21" t="s">
         <v>301</v>
@@ -2925,7 +2912,7 @@
         <v>58</v>
       </c>
       <c r="X12" s="21" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="13" spans="1:30" ht="57.75" x14ac:dyDescent="0.25">
@@ -2979,7 +2966,7 @@
         <v>58</v>
       </c>
       <c r="X13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="14" spans="1:30" ht="57.75" x14ac:dyDescent="0.25">
@@ -3080,10 +3067,10 @@
         <v>306</v>
       </c>
       <c r="AA15" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="AB15" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -3197,10 +3184,10 @@
         <v>311</v>
       </c>
       <c r="AA17" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="AB17" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
@@ -3314,10 +3301,10 @@
         <v>311</v>
       </c>
       <c r="AA19" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="AB19" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
@@ -3822,7 +3809,7 @@
         <v>330</v>
       </c>
       <c r="X29" s="21" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
@@ -3877,10 +3864,10 @@
         <v>333</v>
       </c>
       <c r="AA30" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="AB30" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
@@ -4031,16 +4018,16 @@
         <v>43</v>
       </c>
       <c r="X33" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="Y33" t="s">
         <v>339</v>
       </c>
       <c r="AA33" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="AB33" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.25">
@@ -4351,7 +4338,7 @@
         <v>353</v>
       </c>
       <c r="X39" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
@@ -4450,7 +4437,7 @@
         <v>353</v>
       </c>
       <c r="X41" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="42" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4525,7 +4512,7 @@
         <v>356</v>
       </c>
       <c r="K43" s="12" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="L43" s="3"/>
       <c r="M43" s="9"/>
@@ -4534,11 +4521,11 @@
         <v>417</v>
       </c>
       <c r="Q43" s="16" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="R43" s="16"/>
       <c r="S43" s="16" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="T43" s="3" t="s">
         <v>24</v>
@@ -4550,16 +4537,16 @@
         <v>32</v>
       </c>
       <c r="W43" t="s">
+        <v>447</v>
+      </c>
+      <c r="X43" t="s">
+        <v>448</v>
+      </c>
+      <c r="Y43" s="21" t="s">
         <v>449</v>
       </c>
-      <c r="X43" t="s">
+      <c r="AA43" t="s">
         <v>450</v>
-      </c>
-      <c r="Y43" s="21" t="s">
-        <v>451</v>
-      </c>
-      <c r="AA43" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="44" spans="1:28" ht="90" x14ac:dyDescent="0.25">
@@ -4584,13 +4571,13 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="9" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="J44" s="12" t="s">
         <v>357</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="L44" s="3"/>
       <c r="M44" s="9" t="s">
@@ -4692,7 +4679,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="9" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="J46" s="12" t="s">
         <v>361</v>
@@ -4911,7 +4898,7 @@
         <v>363</v>
       </c>
       <c r="S50" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="T50" s="3" t="s">
         <v>24</v>
@@ -5277,7 +5264,7 @@
         <v>201</v>
       </c>
       <c r="W57" s="21" t="s">
-        <v>456</v>
+        <v>467</v>
       </c>
     </row>
     <row r="58" spans="1:23" ht="25.5" x14ac:dyDescent="0.25">
@@ -5761,7 +5748,7 @@
         <v>201</v>
       </c>
       <c r="W68" s="21" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="69" spans="1:28" ht="72" x14ac:dyDescent="0.25">
@@ -5816,7 +5803,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="1:28" ht="375" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28" ht="315" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -5863,10 +5850,10 @@
         <v>201</v>
       </c>
       <c r="W70" s="21" t="s">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="X70" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="71" spans="1:28" ht="51" x14ac:dyDescent="0.25">
@@ -6004,10 +5991,10 @@
         <v>394</v>
       </c>
       <c r="AA73" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="AB73" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="74" spans="1:28" ht="38.25" x14ac:dyDescent="0.25">
@@ -6337,7 +6324,7 @@
         <v>401</v>
       </c>
       <c r="X80" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="81" spans="1:26" ht="25.5" x14ac:dyDescent="0.25">
@@ -6436,10 +6423,10 @@
         <v>58</v>
       </c>
       <c r="X82" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="Z82" s="21" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.25">
@@ -6535,5 +6522,6 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>